<commit_message>
Cambios tipos de calendarios para circuito
</commit_message>
<xml_diff>
--- a/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
+++ b/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
@@ -5,18 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\GESTIÓN CTAPA\03 Temporada 2022-2023\Voley playa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srcRepository\Proyectos Estela\Federacion\VoleyPlaya.GestionWeb\wwwroot\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9E3F0C-1311-4C2C-A389-447DB4DB222A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{484D2709-9A25-401E-93B2-98A116D42E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D623535B-36BD-4D0F-9B7E-7EE7C623A758}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{D623535B-36BD-4D0F-9B7E-7EE7C623A758}"/>
   </bookViews>
   <sheets>
     <sheet name="8 EQUIPOS" sheetId="1" r:id="rId1"/>
     <sheet name="12 EQUIPOS" sheetId="2" r:id="rId2"/>
     <sheet name="16 EQUIPOS" sheetId="3" r:id="rId3"/>
     <sheet name="24 EQUIPOS" sheetId="4" r:id="rId4"/>
+    <sheet name="1 GRUPOS" sheetId="7" r:id="rId5"/>
+    <sheet name="2 GRUPOS" sheetId="6" r:id="rId6"/>
+    <sheet name="4 GRUPOS" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="54">
   <si>
     <t>Partido</t>
   </si>
@@ -150,6 +153,57 @@
   </si>
   <si>
     <t>GP22</t>
+  </si>
+  <si>
+    <t>Jornada</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>2C</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>3D</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>PP3</t>
+  </si>
+  <si>
+    <t>PP4</t>
   </si>
 </sst>
 </file>
@@ -185,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,6 +250,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,13 +568,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7482AF-665B-4A24-9804-D7B1DC81A9A2}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,8 +589,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -543,8 +606,11 @@
       <c r="D2" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -557,8 +623,11 @@
       <c r="D3" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -571,8 +640,11 @@
       <c r="D4" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -585,8 +657,11 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -599,8 +674,11 @@
       <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -613,8 +691,11 @@
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -627,8 +708,11 @@
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -640,6 +724,9 @@
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -649,15 +736,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656B6CC3-C917-4222-823E-6D16BA8F3290}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D13"/>
+      <selection activeCell="E1" sqref="E1:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,8 +757,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -684,8 +774,11 @@
       <c r="D2" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -698,8 +791,11 @@
       <c r="D3" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -712,8 +808,11 @@
       <c r="D4" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -726,8 +825,11 @@
       <c r="D5" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -740,8 +842,11 @@
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -754,8 +859,11 @@
       <c r="D7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -768,8 +876,11 @@
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -782,8 +893,11 @@
       <c r="D9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -796,8 +910,11 @@
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -810,8 +927,11 @@
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -824,8 +944,11 @@
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -837,6 +960,9 @@
       </c>
       <c r="D13" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -846,15 +972,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCF2F7A-2918-42F7-836B-FE775AC17E67}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D17"/>
+      <selection activeCell="E1" sqref="E1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,8 +993,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -881,8 +1010,11 @@
       <c r="D2" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -895,8 +1027,11 @@
       <c r="D3" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -909,8 +1044,11 @@
       <c r="D4" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -923,8 +1061,11 @@
       <c r="D5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -937,8 +1078,11 @@
       <c r="D6" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -951,8 +1095,11 @@
       <c r="D7" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -965,8 +1112,11 @@
       <c r="D8" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -979,8 +1129,11 @@
       <c r="D9" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -993,8 +1146,11 @@
       <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1007,8 +1163,11 @@
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1021,8 +1180,11 @@
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1035,8 +1197,11 @@
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1049,8 +1214,11 @@
       <c r="D14" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1063,8 +1231,11 @@
       <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1077,8 +1248,11 @@
       <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1090,6 +1264,9 @@
       </c>
       <c r="D17" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1099,15 +1276,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F5A38C-8E6B-497D-9F29-334DAAF34C15}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1120,8 +1297,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1134,8 +1314,11 @@
       <c r="D2" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1148,8 +1331,11 @@
       <c r="D3" s="1">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1162,8 +1348,11 @@
       <c r="D4" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1176,8 +1365,11 @@
       <c r="D5" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1190,8 +1382,11 @@
       <c r="D6" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1204,8 +1399,11 @@
       <c r="D7" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1218,8 +1416,11 @@
       <c r="D8" s="1">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1232,8 +1433,11 @@
       <c r="D9" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1246,8 +1450,11 @@
       <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1260,8 +1467,11 @@
       <c r="D11" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1274,8 +1484,11 @@
       <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1288,8 +1501,11 @@
       <c r="D13" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1302,8 +1518,11 @@
       <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1316,8 +1535,11 @@
       <c r="D15" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1330,8 +1552,11 @@
       <c r="D16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1344,8 +1569,11 @@
       <c r="D17" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1358,8 +1586,11 @@
       <c r="D18" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1372,8 +1603,11 @@
       <c r="D19" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1386,8 +1620,11 @@
       <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1400,8 +1637,11 @@
       <c r="D21" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1414,8 +1654,11 @@
       <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1428,8 +1671,11 @@
       <c r="D23" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1442,8 +1688,11 @@
       <c r="D24" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1455,6 +1704,446 @@
       </c>
       <c r="D25" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="E25" s="1">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E939826B-AA9A-4901-8050-976450D53374}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1675D1B4-BFC5-42B3-A2E4-4D88E6AB00BA}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C3399-4F00-43DE-8297-E4D50E3DA5A6}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gestion de fases finales
</commit_message>
<xml_diff>
--- a/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
+++ b/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srcRepository\Proyectos Estela\Federacion\VoleyPlaya.GestionWeb\wwwroot\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{484D2709-9A25-401E-93B2-98A116D42E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B7CD57-DB07-4359-8550-015B854F8883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{D623535B-36BD-4D0F-9B7E-7EE7C623A758}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{D623535B-36BD-4D0F-9B7E-7EE7C623A758}"/>
   </bookViews>
   <sheets>
     <sheet name="8 EQUIPOS" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="24 EQUIPOS" sheetId="4" r:id="rId4"/>
     <sheet name="1 GRUPOS" sheetId="7" r:id="rId5"/>
     <sheet name="2 GRUPOS" sheetId="6" r:id="rId6"/>
-    <sheet name="4 GRUPOS" sheetId="5" r:id="rId7"/>
+    <sheet name="3 GRUPOS" sheetId="8" r:id="rId7"/>
+    <sheet name="4 GRUPOS" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="57">
   <si>
     <t>Partido</t>
   </si>
@@ -204,6 +205,15 @@
   </si>
   <si>
     <t>PP4</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>PP7</t>
+  </si>
+  <si>
+    <t>PP8</t>
   </si>
 </sst>
 </file>
@@ -1916,11 +1926,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C3399-4F00-43DE-8297-E4D50E3DA5A6}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36573007-E032-4D71-8461-F75D329C90BA}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,6 +1960,208 @@
         <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C3399-4F00-43DE-8297-E4D50E3DA5A6}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D2" s="1" t="s">

</xml_diff>

<commit_message>
Añadida la prueba como clave de una competición Añadida clasificación de grupos en Edicion Añadida clasificación final en edición
</commit_message>
<xml_diff>
--- a/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
+++ b/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srcRepository\Proyectos Estela\Federacion\VoleyPlaya.GestionWeb\wwwroot\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B7CD57-DB07-4359-8550-015B854F8883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{D623535B-36BD-4D0F-9B7E-7EE7C623A758}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="8 EQUIPOS" sheetId="1" r:id="rId1"/>
@@ -22,9 +16,9 @@
     <sheet name="3 GRUPOS" sheetId="8" r:id="rId7"/>
     <sheet name="4 GRUPOS" sheetId="5" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="60">
   <si>
     <t>Partido</t>
   </si>
@@ -214,13 +208,22 @@
   </si>
   <si>
     <t>PP8</t>
+  </si>
+  <si>
+    <t>´1/4</t>
+  </si>
+  <si>
+    <t>´1/8</t>
+  </si>
+  <si>
+    <t>`1/4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -264,6 +267,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -324,7 +330,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -376,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -570,23 +576,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C7482AF-665B-4A24-9804-D7B1DC81A9A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,7 +609,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -620,7 +626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -637,7 +643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -654,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -671,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -688,7 +694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -705,7 +711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -722,7 +728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -745,16 +751,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656B6CC3-C917-4222-823E-6D16BA8F3290}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -788,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -805,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -822,7 +828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -839,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -856,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -873,7 +879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -890,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -907,7 +913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -924,7 +930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -941,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -958,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -981,16 +987,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFCF2F7A-2918-42F7-836B-FE775AC17E67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1024,7 +1030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1058,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1075,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1092,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1143,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1160,7 +1166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1177,7 +1183,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1211,7 +1217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1228,7 +1234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1245,7 +1251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1285,16 +1291,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F5A38C-8E6B-497D-9F29-334DAAF34C15}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1328,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1345,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1362,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1379,7 +1385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1396,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1413,7 +1419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1430,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1447,7 +1453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1464,7 +1470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1498,7 +1504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1515,7 +1521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1532,7 +1538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1600,7 +1606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1617,7 +1623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1651,7 +1657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1685,7 +1691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1702,7 +1708,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1726,16 +1732,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E939826B-AA9A-4901-8050-976450D53374}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1752,7 +1758,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1769,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1792,16 +1798,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1675D1B4-BFC5-42B3-A2E4-4D88E6AB00BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1818,7 +1824,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1835,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1863,30 +1869,30 @@
         <v>47</v>
       </c>
       <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
         <v>49</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
       <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1903,7 +1909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1926,16 +1932,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36573007-E032-4D71-8461-F75D329C90BA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1952,12 +1958,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>38</v>
+      <c r="B2" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
@@ -1969,12 +1975,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>42</v>
@@ -1986,75 +1992,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>38</v>
+      <c r="B7" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2065,13 +2071,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2079,16 +2085,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2105,7 +2111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2128,16 +2134,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C3399-4F00-43DE-8297-E4D50E3DA5A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2154,12 +2160,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>39</v>
@@ -2171,12 +2177,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>41</v>
@@ -2188,12 +2194,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>43</v>
@@ -2205,12 +2211,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>45</v>
@@ -2222,12 +2228,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>47</v>
@@ -2239,12 +2245,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>48</v>
@@ -2256,12 +2262,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>49</v>
@@ -2273,12 +2279,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>50</v>
@@ -2290,7 +2296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2307,7 +2313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2341,7 +2347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
resultados con usuario y validador generación de 2 grupos en semilla más arreglos
</commit_message>
<xml_diff>
--- a/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
+++ b/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srcRepository\Proyectos Estela\Federacion\VoleyPlaya.GestionWeb\wwwroot\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441B234C-E8E3-4F46-A135-3A1E156442FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="8 EQUIPOS" sheetId="1" r:id="rId1"/>
@@ -17,27 +23,16 @@
     <sheet name="4 GRUPOS" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="58">
   <si>
     <t>Partido</t>
   </si>
@@ -153,9 +148,6 @@
     <t>Jornada</t>
   </si>
   <si>
-    <t>FF</t>
-  </si>
-  <si>
     <t>2B</t>
   </si>
   <si>
@@ -210,23 +202,26 @@
     <t>PP8</t>
   </si>
   <si>
-    <t>´1/4</t>
-  </si>
-  <si>
-    <t>´1/8</t>
-  </si>
-  <si>
-    <t>`1/4</t>
+    <t>1/4</t>
+  </si>
+  <si>
+    <t>1/8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -252,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,9 +262,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,23 +568,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +601,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -626,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -643,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -660,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -677,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -694,7 +686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -711,7 +703,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -728,7 +720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -751,16 +743,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -777,7 +769,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -794,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -811,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -828,7 +820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -845,7 +837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -862,7 +854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -879,7 +871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -896,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -913,7 +905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -930,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -947,7 +939,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -964,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -987,16 +979,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1030,7 +1022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1047,7 +1039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1064,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1081,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1098,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1115,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1132,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1149,7 +1141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1166,7 +1158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1183,7 +1175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1200,7 +1192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1217,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1234,7 +1226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1251,7 +1243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1268,7 +1260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1291,16 +1283,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1317,7 +1309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1334,7 +1326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1351,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1368,7 +1360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1385,7 +1377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1402,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1419,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1436,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1453,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1470,7 +1462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1487,7 +1479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1504,7 +1496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1521,7 +1513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1538,7 +1530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1555,7 +1547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1572,7 +1564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1589,7 +1581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1606,7 +1598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1623,7 +1615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1640,7 +1632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1657,7 +1649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1674,7 +1666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1691,7 +1683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1708,7 +1700,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1732,16 +1724,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1758,7 +1750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1766,16 +1758,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1783,10 +1775,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -1798,16 +1790,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1824,49 +1816,49 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -1875,7 +1867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1883,7 +1875,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -1892,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1900,16 +1892,16 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
       <c r="E6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1932,16 +1924,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1958,49 +1950,49 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>58</v>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -2009,15 +2001,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>57</v>
+      <c r="B5" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -2026,41 +2018,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>57</v>
+      <c r="B6" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>57</v>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2077,7 +2069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2094,7 +2086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2102,16 +2094,16 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="E10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2129,21 +2121,22 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2160,83 +2153,83 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
+      <c r="B2" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>59</v>
+      <c r="B6" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -2245,15 +2238,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>59</v>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>6</v>
@@ -2262,15 +2255,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>59</v>
+      <c r="B8" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
@@ -2279,15 +2272,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>59</v>
+      <c r="B9" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -2296,7 +2289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2313,7 +2306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2330,7 +2323,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2347,7 +2340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2365,6 +2358,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglar calendario 34 grupos
</commit_message>
<xml_diff>
--- a/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
+++ b/Federacion/VoleyPlaya.GestionWeb/wwwroot/excel/calendarios.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srcRepository\Proyectos Estela\Federacion\VoleyPlaya.GestionWeb\wwwroot\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\srcRepository\ProyectosEstela\Federacion\VoleyPlaya.GestionWeb\wwwroot\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D435C6-9969-4A72-B7FF-EDE7DECA62A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DF692F-89ED-4B46-BCAE-5D4AAA55DF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="254">
   <si>
     <t>Partido</t>
   </si>
@@ -420,9 +420,6 @@
   </si>
   <si>
     <t>3S</t>
-  </si>
-  <si>
-    <t>ST</t>
   </si>
   <si>
     <t>3U</t>
@@ -2544,7 +2541,7 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2561,7 +2558,7 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2779,7 +2776,7 @@
         <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
         <v>41</v>
@@ -2796,7 +2793,7 @@
         <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D17" t="s">
         <v>45</v>
@@ -2816,7 +2813,7 @@
         <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -2833,7 +2830,7 @@
         <v>122</v>
       </c>
       <c r="D19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -2850,7 +2847,7 @@
         <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -2864,10 +2861,10 @@
         <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -2881,10 +2878,10 @@
         <v>70</v>
       </c>
       <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
         <v>125</v>
-      </c>
-      <c r="D22" t="s">
-        <v>126</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2898,10 +2895,10 @@
         <v>70</v>
       </c>
       <c r="C23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" t="s">
         <v>127</v>
-      </c>
-      <c r="D23" t="s">
-        <v>128</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -2915,10 +2912,10 @@
         <v>70</v>
       </c>
       <c r="C24" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" t="s">
         <v>129</v>
-      </c>
-      <c r="D24" t="s">
-        <v>130</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -2932,10 +2929,10 @@
         <v>70</v>
       </c>
       <c r="C25" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" t="s">
         <v>131</v>
-      </c>
-      <c r="D25" t="s">
-        <v>132</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2949,7 +2946,7 @@
         <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -2966,7 +2963,7 @@
         <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -3221,7 +3218,7 @@
         <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D42" t="s">
         <v>30</v>
@@ -3238,7 +3235,7 @@
         <v>69</v>
       </c>
       <c r="C43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D43" t="s">
         <v>29</v>
@@ -3255,7 +3252,7 @@
         <v>69</v>
       </c>
       <c r="C44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
         <v>32</v>
@@ -3272,7 +3269,7 @@
         <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D45" t="s">
         <v>31</v>
@@ -3289,7 +3286,7 @@
         <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
         <v>36</v>
@@ -3306,7 +3303,7 @@
         <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D47" t="s">
         <v>35</v>
@@ -3323,7 +3320,7 @@
         <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D48" t="s">
         <v>96</v>
@@ -3340,7 +3337,7 @@
         <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D49" t="s">
         <v>95</v>
@@ -3357,10 +3354,10 @@
         <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -3374,10 +3371,10 @@
         <v>69</v>
       </c>
       <c r="C51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -3391,10 +3388,10 @@
         <v>69</v>
       </c>
       <c r="C52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E52">
         <v>0</v>
@@ -3408,10 +3405,10 @@
         <v>69</v>
       </c>
       <c r="C53" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D53" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -3425,10 +3422,10 @@
         <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D54" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -3442,10 +3439,10 @@
         <v>69</v>
       </c>
       <c r="C55" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D55" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -3459,10 +3456,10 @@
         <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -3476,10 +3473,10 @@
         <v>69</v>
       </c>
       <c r="C57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D57" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -3615,7 +3612,7 @@
         <v>111</v>
       </c>
       <c r="D65" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -3646,10 +3643,10 @@
         <v>57</v>
       </c>
       <c r="C67" t="s">
+        <v>182</v>
+      </c>
+      <c r="D67" t="s">
         <v>183</v>
-      </c>
-      <c r="D67" t="s">
-        <v>184</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -3663,10 +3660,10 @@
         <v>57</v>
       </c>
       <c r="C68" t="s">
+        <v>184</v>
+      </c>
+      <c r="D68" t="s">
         <v>185</v>
-      </c>
-      <c r="D68" t="s">
-        <v>186</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -3680,10 +3677,10 @@
         <v>57</v>
       </c>
       <c r="C69" t="s">
+        <v>186</v>
+      </c>
+      <c r="D69" t="s">
         <v>187</v>
-      </c>
-      <c r="D69" t="s">
-        <v>188</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -3697,10 +3694,10 @@
         <v>57</v>
       </c>
       <c r="C70" t="s">
+        <v>188</v>
+      </c>
+      <c r="D70" t="s">
         <v>189</v>
-      </c>
-      <c r="D70" t="s">
-        <v>190</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -3714,10 +3711,10 @@
         <v>57</v>
       </c>
       <c r="C71" t="s">
+        <v>190</v>
+      </c>
+      <c r="D71" t="s">
         <v>191</v>
-      </c>
-      <c r="D71" t="s">
-        <v>192</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -3731,10 +3728,10 @@
         <v>57</v>
       </c>
       <c r="C72" t="s">
+        <v>192</v>
+      </c>
+      <c r="D72" t="s">
         <v>193</v>
-      </c>
-      <c r="D72" t="s">
-        <v>194</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -3748,10 +3745,10 @@
         <v>57</v>
       </c>
       <c r="C73" t="s">
+        <v>194</v>
+      </c>
+      <c r="D73" t="s">
         <v>195</v>
-      </c>
-      <c r="D73" t="s">
-        <v>196</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -3765,10 +3762,10 @@
         <v>56</v>
       </c>
       <c r="C74" t="s">
+        <v>196</v>
+      </c>
+      <c r="D74" t="s">
         <v>197</v>
-      </c>
-      <c r="D74" t="s">
-        <v>198</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -3782,10 +3779,10 @@
         <v>56</v>
       </c>
       <c r="C75" t="s">
+        <v>198</v>
+      </c>
+      <c r="D75" t="s">
         <v>199</v>
-      </c>
-      <c r="D75" t="s">
-        <v>200</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -3799,10 +3796,10 @@
         <v>56</v>
       </c>
       <c r="C76" t="s">
+        <v>200</v>
+      </c>
+      <c r="D76" t="s">
         <v>201</v>
-      </c>
-      <c r="D76" t="s">
-        <v>202</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -3816,10 +3813,10 @@
         <v>56</v>
       </c>
       <c r="C77" t="s">
+        <v>202</v>
+      </c>
+      <c r="D77" t="s">
         <v>203</v>
-      </c>
-      <c r="D77" t="s">
-        <v>204</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -3833,10 +3830,10 @@
         <v>56</v>
       </c>
       <c r="C78" t="s">
+        <v>204</v>
+      </c>
+      <c r="D78" t="s">
         <v>205</v>
-      </c>
-      <c r="D78" t="s">
-        <v>206</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -3850,10 +3847,10 @@
         <v>56</v>
       </c>
       <c r="C79" t="s">
+        <v>206</v>
+      </c>
+      <c r="D79" t="s">
         <v>207</v>
-      </c>
-      <c r="D79" t="s">
-        <v>208</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -3867,10 +3864,10 @@
         <v>56</v>
       </c>
       <c r="C80" t="s">
+        <v>208</v>
+      </c>
+      <c r="D80" t="s">
         <v>209</v>
-      </c>
-      <c r="D80" t="s">
-        <v>210</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -3884,10 +3881,10 @@
         <v>56</v>
       </c>
       <c r="C81" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D81" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -3901,10 +3898,10 @@
         <v>55</v>
       </c>
       <c r="C82" t="s">
+        <v>213</v>
+      </c>
+      <c r="D82" t="s">
         <v>214</v>
-      </c>
-      <c r="D82" t="s">
-        <v>215</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -3918,10 +3915,10 @@
         <v>55</v>
       </c>
       <c r="C83" t="s">
+        <v>215</v>
+      </c>
+      <c r="D83" t="s">
         <v>216</v>
-      </c>
-      <c r="D83" t="s">
-        <v>217</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -3935,10 +3932,10 @@
         <v>55</v>
       </c>
       <c r="C84" t="s">
+        <v>217</v>
+      </c>
+      <c r="D84" t="s">
         <v>218</v>
-      </c>
-      <c r="D84" t="s">
-        <v>219</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -3952,10 +3949,10 @@
         <v>55</v>
       </c>
       <c r="C85" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -3969,10 +3966,10 @@
         <v>4</v>
       </c>
       <c r="C86" t="s">
+        <v>221</v>
+      </c>
+      <c r="D86" t="s">
         <v>222</v>
-      </c>
-      <c r="D86" t="s">
-        <v>223</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -3986,10 +3983,10 @@
         <v>4</v>
       </c>
       <c r="C87" t="s">
+        <v>223</v>
+      </c>
+      <c r="D87" t="s">
         <v>224</v>
-      </c>
-      <c r="D87" t="s">
-        <v>225</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -4003,10 +4000,10 @@
         <v>9</v>
       </c>
       <c r="C88" t="s">
+        <v>250</v>
+      </c>
+      <c r="D88" t="s">
         <v>251</v>
-      </c>
-      <c r="D88" t="s">
-        <v>252</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -4020,10 +4017,10 @@
         <v>62</v>
       </c>
       <c r="C89" t="s">
+        <v>225</v>
+      </c>
+      <c r="D89" t="s">
         <v>226</v>
-      </c>
-      <c r="D89" t="s">
-        <v>227</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -4039,8 +4036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC351E8-F8EA-42D6-BFC3-4BF49988FFAD}">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4070,7 +4067,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C2" t="s">
         <v>121</v>
@@ -4087,13 +4084,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C3" t="s">
         <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>247</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -4104,13 +4101,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
         <v>125</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -4121,13 +4118,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" t="s">
         <v>127</v>
-      </c>
-      <c r="D5" t="s">
-        <v>128</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4138,13 +4135,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" t="s">
         <v>129</v>
-      </c>
-      <c r="D6" t="s">
-        <v>130</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -4155,13 +4152,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
         <v>131</v>
-      </c>
-      <c r="D7" t="s">
-        <v>132</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -4172,13 +4169,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
         <v>133</v>
-      </c>
-      <c r="D8" t="s">
-        <v>134</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -4189,13 +4186,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" t="s">
         <v>135</v>
-      </c>
-      <c r="D9" t="s">
-        <v>136</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -4206,13 +4203,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" t="s">
         <v>137</v>
-      </c>
-      <c r="D10" t="s">
-        <v>138</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -4229,7 +4226,7 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -4246,7 +4243,7 @@
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -4464,7 +4461,7 @@
         <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D25" t="s">
         <v>41</v>
@@ -4481,7 +4478,7 @@
         <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D26" t="s">
         <v>45</v>
@@ -4498,10 +4495,10 @@
         <v>70</v>
       </c>
       <c r="C27" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" t="s">
         <v>143</v>
-      </c>
-      <c r="D27" t="s">
-        <v>144</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4515,10 +4512,10 @@
         <v>70</v>
       </c>
       <c r="C28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" t="s">
         <v>145</v>
-      </c>
-      <c r="D28" t="s">
-        <v>146</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -4532,10 +4529,10 @@
         <v>70</v>
       </c>
       <c r="C29" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" t="s">
         <v>147</v>
-      </c>
-      <c r="D29" t="s">
-        <v>148</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4549,10 +4546,10 @@
         <v>70</v>
       </c>
       <c r="C30" t="s">
+        <v>148</v>
+      </c>
+      <c r="D30" t="s">
         <v>149</v>
-      </c>
-      <c r="D30" t="s">
-        <v>150</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -4566,7 +4563,7 @@
         <v>70</v>
       </c>
       <c r="C31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
@@ -4583,7 +4580,7 @@
         <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -4600,7 +4597,7 @@
         <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -4617,7 +4614,7 @@
         <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
@@ -4634,7 +4631,7 @@
         <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -4651,7 +4648,7 @@
         <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
@@ -4668,7 +4665,7 @@
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -4685,7 +4682,7 @@
         <v>70</v>
       </c>
       <c r="C38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
@@ -4702,10 +4699,10 @@
         <v>70</v>
       </c>
       <c r="C39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" t="s">
         <v>159</v>
-      </c>
-      <c r="D39" t="s">
-        <v>160</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -4719,10 +4716,10 @@
         <v>70</v>
       </c>
       <c r="C40" t="s">
+        <v>160</v>
+      </c>
+      <c r="D40" t="s">
         <v>161</v>
-      </c>
-      <c r="D40" t="s">
-        <v>162</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -4974,7 +4971,7 @@
         <v>69</v>
       </c>
       <c r="C55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
         <v>20</v>
@@ -4991,7 +4988,7 @@
         <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D56" t="s">
         <v>21</v>
@@ -5008,10 +5005,10 @@
         <v>69</v>
       </c>
       <c r="C57" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" t="s">
         <v>165</v>
-      </c>
-      <c r="D57" t="s">
-        <v>166</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -5025,10 +5022,10 @@
         <v>69</v>
       </c>
       <c r="C58" t="s">
+        <v>166</v>
+      </c>
+      <c r="D58" t="s">
         <v>167</v>
-      </c>
-      <c r="D58" t="s">
-        <v>168</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -5042,7 +5039,7 @@
         <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D59" t="s">
         <v>98</v>
@@ -5059,7 +5056,7 @@
         <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D60" t="s">
         <v>99</v>
@@ -5076,7 +5073,7 @@
         <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D61" t="s">
         <v>100</v>
@@ -5093,7 +5090,7 @@
         <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D62" t="s">
         <v>101</v>
@@ -5110,7 +5107,7 @@
         <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D63" t="s">
         <v>102</v>
@@ -5127,7 +5124,7 @@
         <v>69</v>
       </c>
       <c r="C64" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D64" t="s">
         <v>103</v>
@@ -5144,7 +5141,7 @@
         <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D65" t="s">
         <v>104</v>
@@ -5161,7 +5158,7 @@
         <v>69</v>
       </c>
       <c r="C66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D66" t="s">
         <v>105</v>
@@ -5178,7 +5175,7 @@
         <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D67" t="s">
         <v>106</v>
@@ -5195,7 +5192,7 @@
         <v>69</v>
       </c>
       <c r="C68" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D68" t="s">
         <v>107</v>
@@ -5212,7 +5209,7 @@
         <v>69</v>
       </c>
       <c r="C69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D69" t="s">
         <v>108</v>
@@ -5229,7 +5226,7 @@
         <v>69</v>
       </c>
       <c r="C70" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D70" t="s">
         <v>109</v>
@@ -5246,7 +5243,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D71" t="s">
         <v>110</v>
@@ -5263,7 +5260,7 @@
         <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D72" t="s">
         <v>111</v>
@@ -5300,7 +5297,7 @@
         <v>116</v>
       </c>
       <c r="D74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -5314,10 +5311,10 @@
         <v>57</v>
       </c>
       <c r="C75" t="s">
+        <v>183</v>
+      </c>
+      <c r="D75" t="s">
         <v>184</v>
-      </c>
-      <c r="D75" t="s">
-        <v>185</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -5331,10 +5328,10 @@
         <v>57</v>
       </c>
       <c r="C76" t="s">
+        <v>185</v>
+      </c>
+      <c r="D76" t="s">
         <v>186</v>
-      </c>
-      <c r="D76" t="s">
-        <v>187</v>
       </c>
       <c r="E76">
         <v>0</v>
@@ -5348,10 +5345,10 @@
         <v>57</v>
       </c>
       <c r="C77" t="s">
+        <v>187</v>
+      </c>
+      <c r="D77" t="s">
         <v>188</v>
-      </c>
-      <c r="D77" t="s">
-        <v>189</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -5365,10 +5362,10 @@
         <v>57</v>
       </c>
       <c r="C78" t="s">
+        <v>189</v>
+      </c>
+      <c r="D78" t="s">
         <v>190</v>
-      </c>
-      <c r="D78" t="s">
-        <v>191</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -5382,10 +5379,10 @@
         <v>57</v>
       </c>
       <c r="C79" t="s">
+        <v>191</v>
+      </c>
+      <c r="D79" t="s">
         <v>192</v>
-      </c>
-      <c r="D79" t="s">
-        <v>193</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -5399,10 +5396,10 @@
         <v>57</v>
       </c>
       <c r="C80" t="s">
+        <v>193</v>
+      </c>
+      <c r="D80" t="s">
         <v>194</v>
-      </c>
-      <c r="D80" t="s">
-        <v>195</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -5416,10 +5413,10 @@
         <v>57</v>
       </c>
       <c r="C81" t="s">
+        <v>195</v>
+      </c>
+      <c r="D81" t="s">
         <v>196</v>
-      </c>
-      <c r="D81" t="s">
-        <v>197</v>
       </c>
       <c r="E81">
         <v>0</v>
@@ -5433,10 +5430,10 @@
         <v>57</v>
       </c>
       <c r="C82" t="s">
+        <v>197</v>
+      </c>
+      <c r="D82" t="s">
         <v>198</v>
-      </c>
-      <c r="D82" t="s">
-        <v>199</v>
       </c>
       <c r="E82">
         <v>0</v>
@@ -5450,10 +5447,10 @@
         <v>57</v>
       </c>
       <c r="C83" t="s">
+        <v>199</v>
+      </c>
+      <c r="D83" t="s">
         <v>200</v>
-      </c>
-      <c r="D83" t="s">
-        <v>201</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -5467,10 +5464,10 @@
         <v>57</v>
       </c>
       <c r="C84" t="s">
+        <v>201</v>
+      </c>
+      <c r="D84" t="s">
         <v>202</v>
-      </c>
-      <c r="D84" t="s">
-        <v>203</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -5484,10 +5481,10 @@
         <v>57</v>
       </c>
       <c r="C85" t="s">
+        <v>203</v>
+      </c>
+      <c r="D85" t="s">
         <v>204</v>
-      </c>
-      <c r="D85" t="s">
-        <v>205</v>
       </c>
       <c r="E85">
         <v>0</v>
@@ -5501,10 +5498,10 @@
         <v>57</v>
       </c>
       <c r="C86" t="s">
+        <v>205</v>
+      </c>
+      <c r="D86" t="s">
         <v>206</v>
-      </c>
-      <c r="D86" t="s">
-        <v>207</v>
       </c>
       <c r="E86">
         <v>0</v>
@@ -5518,10 +5515,10 @@
         <v>57</v>
       </c>
       <c r="C87" t="s">
+        <v>207</v>
+      </c>
+      <c r="D87" t="s">
         <v>208</v>
-      </c>
-      <c r="D87" t="s">
-        <v>209</v>
       </c>
       <c r="E87">
         <v>0</v>
@@ -5535,10 +5532,10 @@
         <v>57</v>
       </c>
       <c r="C88" t="s">
+        <v>209</v>
+      </c>
+      <c r="D88" t="s">
         <v>210</v>
-      </c>
-      <c r="D88" t="s">
-        <v>211</v>
       </c>
       <c r="E88">
         <v>0</v>
@@ -5552,10 +5549,10 @@
         <v>56</v>
       </c>
       <c r="C89" t="s">
+        <v>212</v>
+      </c>
+      <c r="D89" t="s">
         <v>213</v>
-      </c>
-      <c r="D89" t="s">
-        <v>214</v>
       </c>
       <c r="E89">
         <v>0</v>
@@ -5569,10 +5566,10 @@
         <v>56</v>
       </c>
       <c r="C90" t="s">
+        <v>214</v>
+      </c>
+      <c r="D90" t="s">
         <v>215</v>
-      </c>
-      <c r="D90" t="s">
-        <v>216</v>
       </c>
       <c r="E90">
         <v>0</v>
@@ -5586,10 +5583,10 @@
         <v>56</v>
       </c>
       <c r="C91" t="s">
+        <v>216</v>
+      </c>
+      <c r="D91" t="s">
         <v>217</v>
-      </c>
-      <c r="D91" t="s">
-        <v>218</v>
       </c>
       <c r="E91">
         <v>0</v>
@@ -5603,10 +5600,10 @@
         <v>56</v>
       </c>
       <c r="C92" t="s">
+        <v>218</v>
+      </c>
+      <c r="D92" t="s">
         <v>219</v>
-      </c>
-      <c r="D92" t="s">
-        <v>220</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -5620,10 +5617,10 @@
         <v>56</v>
       </c>
       <c r="C93" t="s">
+        <v>220</v>
+      </c>
+      <c r="D93" t="s">
         <v>221</v>
-      </c>
-      <c r="D93" t="s">
-        <v>222</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -5637,10 +5634,10 @@
         <v>56</v>
       </c>
       <c r="C94" t="s">
+        <v>222</v>
+      </c>
+      <c r="D94" t="s">
         <v>223</v>
-      </c>
-      <c r="D94" t="s">
-        <v>224</v>
       </c>
       <c r="E94">
         <v>0</v>
@@ -5654,10 +5651,10 @@
         <v>56</v>
       </c>
       <c r="C95" t="s">
+        <v>224</v>
+      </c>
+      <c r="D95" t="s">
         <v>225</v>
-      </c>
-      <c r="D95" t="s">
-        <v>226</v>
       </c>
       <c r="E95">
         <v>0</v>
@@ -5671,10 +5668,10 @@
         <v>56</v>
       </c>
       <c r="C96" t="s">
+        <v>226</v>
+      </c>
+      <c r="D96" t="s">
         <v>227</v>
-      </c>
-      <c r="D96" t="s">
-        <v>228</v>
       </c>
       <c r="E96">
         <v>0</v>
@@ -5688,10 +5685,10 @@
         <v>55</v>
       </c>
       <c r="C97" t="s">
+        <v>229</v>
+      </c>
+      <c r="D97" t="s">
         <v>230</v>
-      </c>
-      <c r="D97" t="s">
-        <v>231</v>
       </c>
       <c r="E97">
         <v>0</v>
@@ -5705,10 +5702,10 @@
         <v>55</v>
       </c>
       <c r="C98" t="s">
+        <v>231</v>
+      </c>
+      <c r="D98" t="s">
         <v>232</v>
-      </c>
-      <c r="D98" t="s">
-        <v>233</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -5722,10 +5719,10 @@
         <v>55</v>
       </c>
       <c r="C99" t="s">
+        <v>233</v>
+      </c>
+      <c r="D99" t="s">
         <v>234</v>
-      </c>
-      <c r="D99" t="s">
-        <v>235</v>
       </c>
       <c r="E99">
         <v>0</v>
@@ -5739,10 +5736,10 @@
         <v>55</v>
       </c>
       <c r="C100" t="s">
+        <v>235</v>
+      </c>
+      <c r="D100" t="s">
         <v>236</v>
-      </c>
-      <c r="D100" t="s">
-        <v>237</v>
       </c>
       <c r="E100">
         <v>0</v>
@@ -5756,10 +5753,10 @@
         <v>4</v>
       </c>
       <c r="C101" t="s">
+        <v>237</v>
+      </c>
+      <c r="D101" t="s">
         <v>238</v>
-      </c>
-      <c r="D101" t="s">
-        <v>239</v>
       </c>
       <c r="E101">
         <v>0</v>
@@ -5773,10 +5770,10 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
+        <v>239</v>
+      </c>
+      <c r="D102" t="s">
         <v>240</v>
-      </c>
-      <c r="D102" t="s">
-        <v>241</v>
       </c>
       <c r="E102">
         <v>0</v>
@@ -5790,10 +5787,10 @@
         <v>9</v>
       </c>
       <c r="C103" t="s">
+        <v>242</v>
+      </c>
+      <c r="D103" t="s">
         <v>243</v>
-      </c>
-      <c r="D103" t="s">
-        <v>244</v>
       </c>
       <c r="E103">
         <v>0</v>
@@ -5807,10 +5804,10 @@
         <v>62</v>
       </c>
       <c r="C104" t="s">
+        <v>244</v>
+      </c>
+      <c r="D104" t="s">
         <v>245</v>
-      </c>
-      <c r="D104" t="s">
-        <v>246</v>
       </c>
       <c r="E104">
         <v>0</v>
@@ -7035,7 +7032,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -7053,7 +7050,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -7070,7 +7067,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -7087,7 +7084,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
@@ -7104,7 +7101,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
@@ -7121,7 +7118,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" t="s">
         <v>42</v>
@@ -7172,7 +7169,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C10" t="s">
         <v>53</v>
@@ -7196,7 +7193,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>

</xml_diff>